<commit_message>
Updated test form and ZIP file
</commit_message>
<xml_diff>
--- a/extras/test-form/Timed advance.xlsx
+++ b/extras/test-form/Timed advance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B385EF-1A6A-7A46-B39C-13F7E2AE9E53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED328F7-21FE-974A-9027-6CE5E2661F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="424">
   <si>
     <t>type</t>
   </si>
@@ -2657,12 +2657,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>disp</t>
-  </si>
-  <si>
-    <t>custom-timedadvance(duration=5)</t>
-  </si>
-  <si>
     <t>math1</t>
   </si>
   <si>
@@ -2675,28 +2669,12 @@
     <t>12</t>
   </si>
   <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
     <t>select_one math1</t>
   </si>
   <si>
-    <t>math</t>
-  </si>
-  <si>
     <t>quick custom-timedadvance(duration=20)</t>
   </si>
   <si>
-    <t>result</t>
-  </si>
-  <si>
-    <t>if(selected(${math}, '12'), 'Correct', 'Incorrect')</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Name: ${name}&lt;br /&gt;You answered: ${math}&lt;/p&gt;
-&lt;p&gt;You were: ${result}&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p style="font-weight:bold;font-size:24pt;text-align:center;"&gt;3 x 4 = ?&lt;/p&gt;</t>
   </si>
   <si>
@@ -2743,6 +2721,44 @@
   </si>
   <si>
     <t>custom-timedadvance(duration=15, unit='cs')</t>
+  </si>
+  <si>
+    <t>math_int</t>
+  </si>
+  <si>
+    <t>&lt;p style="font-weight:bold;font-size:24pt;text-align:center;"&gt;6 x 3 = ?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>custom-timedadvance(duration=15)</t>
+  </si>
+  <si>
+    <t>result_int</t>
+  </si>
+  <si>
+    <t>disp_int</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You answered: ${math_int}&lt;/p&gt;
+&lt;p&gt;You were: ${result_int}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>math_so</t>
+  </si>
+  <si>
+    <t>result_so</t>
+  </si>
+  <si>
+    <t>if(selected(${math_so}, '12'), 'Correct', 'Incorrect')</t>
+  </si>
+  <si>
+    <t>disp_so</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;You answered: ${math_so}&lt;/p&gt;
+&lt;p&gt;You were: ${result_so}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>if(${math_int} = 18, 'Correct', 'Incorrect')</t>
   </si>
 </sst>
 </file>
@@ -4896,7 +4912,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5163,16 +5179,16 @@
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>412</v>
       </c>
       <c r="C12" t="s">
-        <v>396</v>
+        <v>413</v>
       </c>
       <c r="F12" t="s">
-        <v>391</v>
+        <v>414</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>360</v>
@@ -5184,18 +5200,18 @@
         <v>377</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>397</v>
+        <v>139</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>398</v>
+        <v>415</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>403</v>
+        <v>360</v>
       </c>
       <c r="F13" t="s">
-        <v>399</v>
+        <v>360</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>360</v>
@@ -5204,102 +5220,151 @@
         <v>360</v>
       </c>
       <c r="K13" t="s">
-        <v>377</v>
+        <v>360</v>
+      </c>
+      <c r="N13" t="s">
+        <v>423</v>
       </c>
       <c r="S13" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="K14" t="s">
+        <v>375</v>
+      </c>
+      <c r="N14" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B15" t="s">
+        <v>418</v>
+      </c>
+      <c r="C15" t="s">
+        <v>396</v>
+      </c>
+      <c r="F15" t="s">
+        <v>395</v>
+      </c>
+      <c r="K15" t="s">
+        <v>377</v>
+      </c>
+      <c r="S15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C16" t="s">
         <v>360</v>
       </c>
-      <c r="K14" t="s">
+      <c r="F16" t="s">
         <v>360</v>
       </c>
-      <c r="N14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="K15" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="F16" t="s">
-        <v>418</v>
-      </c>
       <c r="K16" t="s">
-        <v>377</v>
+        <v>360</v>
+      </c>
+      <c r="N16" t="s">
+        <v>420</v>
+      </c>
+      <c r="S16" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>387</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="C17" t="s">
-        <v>412</v>
-      </c>
-      <c r="F17" t="s">
-        <v>378</v>
+        <v>422</v>
       </c>
       <c r="K17" t="s">
-        <v>377</v>
-      </c>
-      <c r="S17" t="s">
-        <v>413</v>
+        <v>375</v>
+      </c>
+      <c r="N17" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>401</v>
       </c>
       <c r="B18" t="s">
-        <v>414</v>
-      </c>
-      <c r="N18" t="s">
-        <v>415</v>
+        <v>403</v>
+      </c>
+      <c r="C18" t="s">
+        <v>402</v>
+      </c>
+      <c r="F18" t="s">
+        <v>411</v>
+      </c>
+      <c r="K18" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>387</v>
+      </c>
+      <c r="B19" t="s">
+        <v>404</v>
+      </c>
+      <c r="C19" t="s">
+        <v>405</v>
+      </c>
+      <c r="F19" t="s">
+        <v>378</v>
+      </c>
+      <c r="K19" t="s">
+        <v>377</v>
+      </c>
+      <c r="S19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>407</v>
+      </c>
+      <c r="N20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s">
-        <v>416</v>
-      </c>
-      <c r="C19" t="s">
-        <v>417</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="B21" t="s">
+        <v>409</v>
+      </c>
+      <c r="C21" t="s">
+        <v>410</v>
+      </c>
+      <c r="K21" t="s">
         <v>375</v>
       </c>
     </row>
@@ -5576,51 +5641,51 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C9" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" t="s">
         <v>392</v>
       </c>
-      <c r="B10" t="s">
-        <v>394</v>
-      </c>
       <c r="C10" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B11" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B12" t="s">
         <v>362</v>
       </c>
       <c r="C12" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B13" t="s">
         <v>388</v>
@@ -5697,7 +5762,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003061243</v>
+        <v>2003091902</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>360</v>

</xml_diff>

<commit_message>
Updated crop list with "None", and set "most" field to only be relevant when "grown" has an actual answer
</commit_message>
<xml_diff>
--- a/extras/test-form/Timed advance.xlsx
+++ b/extras/test-form/Timed advance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED328F7-21FE-974A-9027-6CE5E2661F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4DD964-EACE-AC44-9F8B-5B9AAC2848F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26940" yWindow="540" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="428">
   <si>
     <t>type</t>
   </si>
@@ -2759,6 +2759,18 @@
   </si>
   <si>
     <t>if(${math_int} = 18, 'Correct', 'Incorrect')</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>not(selected(., '0') and count-selected(.) &gt; 1)</t>
+  </si>
+  <si>
+    <t>'None' must be selected by itself!</t>
+  </si>
+  <si>
+    <t>not(selected(${crops_grown}, '-99') or selected(${crops_grown}, '0'))</t>
   </si>
 </sst>
 </file>
@@ -3207,7 +3219,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3323,6 +3335,10 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3356,8 +3372,11 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3471,7 +3490,23 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="134">
+  <dxfs count="135">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4916,7 +4951,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5168,13 +5203,13 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="F11" s="64"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="F11" s="53"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="64"/>
+      <c r="K11" s="53"/>
       <c r="V11"/>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5306,7 +5341,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>401</v>
       </c>
@@ -5318,6 +5353,12 @@
       </c>
       <c r="F18" t="s">
         <v>411</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="H18" s="68" t="s">
+        <v>426</v>
       </c>
       <c r="K18" t="s">
         <v>377</v>
@@ -5335,6 +5376,9 @@
       </c>
       <c r="F19" t="s">
         <v>378</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>427</v>
       </c>
       <c r="K19" t="s">
         <v>377</v>
@@ -5372,137 +5416,137 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="133" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 O1:O1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="132" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="46" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="131" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="43" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="130" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="41" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="129" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="39" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="34" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="127" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="18" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="20" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="22" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="123" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="16" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="122" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="14" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="10" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="120" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="8" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="119" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="2" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="5" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="9" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="11" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="15" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="17" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="19" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="21" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="23" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="25" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="28" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="35" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="40" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="42" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="44" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="45" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="47" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="48" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="50" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5514,11 +5558,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5629,25 +5673,26 @@
       <c r="A8" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="B8" t="s">
-        <v>388</v>
-      </c>
-      <c r="C8" t="s">
-        <v>389</v>
-      </c>
-      <c r="E8" t="s">
-        <v>388</v>
-      </c>
+      <c r="B8" s="67">
+        <v>0</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="B9" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C9" t="s">
-        <v>397</v>
+        <v>389</v>
+      </c>
+      <c r="E9" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5655,10 +5700,10 @@
         <v>390</v>
       </c>
       <c r="B10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5666,10 +5711,10 @@
         <v>390</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5677,10 +5722,10 @@
         <v>390</v>
       </c>
       <c r="B12" t="s">
-        <v>362</v>
+        <v>393</v>
       </c>
       <c r="C12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5688,24 +5733,40 @@
         <v>390</v>
       </c>
       <c r="B13" t="s">
+        <v>362</v>
+      </c>
+      <c r="C13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="B14" t="s">
         <v>388</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="16"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H2000">
-    <cfRule type="expression" dxfId="98" priority="1">
+  <conditionalFormatting sqref="A2:H8 A10:H2001">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>NOT($A2=$A1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:H9">
+    <cfRule type="expression" dxfId="0" priority="100">
+      <formula>NOT($A9=$A7)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5762,7 +5823,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003091902</v>
+        <v>2005041825</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>360</v>
@@ -5797,22 +5858,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6006,10 +6067,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="61" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -6354,7 +6415,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>93</v>
       </c>
@@ -8799,10 +8860,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="63"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -9598,348 +9659,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9962,20 +10023,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10050,28 +10111,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>

<commit_message>
Updated spreadsheet form definition with Arabic
</commit_message>
<xml_diff>
--- a/extras/test-form/Timed advance.xlsx
+++ b/extras/test-form/Timed advance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/timed-advance/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4DD964-EACE-AC44-9F8B-5B9AAC2848F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68FB141-1B56-854A-B922-51298C5ED4F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26940" yWindow="540" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="440">
   <si>
     <t>type</t>
   </si>
@@ -2771,6 +2771,43 @@
   </si>
   <si>
     <t>not(selected(${crops_grown}, '-99') or selected(${crops_grown}, '0'))</t>
+  </si>
+  <si>
+    <t>label:عربى</t>
+  </si>
+  <si>
+    <t>تفاح</t>
+  </si>
+  <si>
+    <t>موز</t>
+  </si>
+  <si>
+    <t>جزر</t>
+  </si>
+  <si>
+    <t>تمور</t>
+  </si>
+  <si>
+    <t>لا يوجد</t>
+  </si>
+  <si>
+    <t>البشري</t>
+  </si>
+  <si>
+    <t>نعم</t>
+  </si>
+  <si>
+    <t>لا</t>
+  </si>
+  <si>
+    <t>ما المحاصيل التي تزرعها؟</t>
+  </si>
+  <si>
+    <t>أي محصول تزرع أكثر؟</t>
+  </si>
+  <si>
+    <t>أنت تنمو أكثر:
+${crop_name}</t>
   </si>
 </sst>
 </file>
@@ -3339,6 +3376,13 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3371,13 +3415,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="108">
@@ -3490,7 +3527,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="136">
     <dxf>
       <font>
         <color auto="1"/>
@@ -4245,6 +4282,22 @@
           <bgColor rgb="FFFFD44B"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4947,11 +5000,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4959,29 +5012,30 @@
     <col min="1" max="1" width="29" style="9" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" style="9" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.33203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.1640625" style="9" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" style="9" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="48" style="9" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="16384" width="11" style="2" collapsed="1"/>
+    <col min="4" max="4" width="30.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.33203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18" style="9" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.33203125" style="9" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.1640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.6640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.5" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15" style="9" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="48" style="9" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="10.83203125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="11" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4991,228 +5045,232 @@
       <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>372</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J2" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V2" t="s">
+      <c r="K2" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J4" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V4" t="s">
+      <c r="K4" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W4" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J5" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V5" t="s">
+      <c r="K5" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W5" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J6" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V6" t="s">
+      <c r="K6" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W6" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J7" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V7" t="s">
+      <c r="K7" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W7" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J8" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V8" t="s">
+      <c r="K8" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W8" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J9" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="K9" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="O9" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>292</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>360</v>
-      </c>
       <c r="J10" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="V10" t="s">
+      <c r="K10" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="W10" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="53"/>
       <c r="B11" s="53"/>
       <c r="C11" s="54"/>
-      <c r="F11" s="53"/>
-      <c r="I11" s="11"/>
+      <c r="D11" s="54"/>
+      <c r="G11" s="53"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="53"/>
-      <c r="V11"/>
-    </row>
-    <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="K11" s="11"/>
+      <c r="L11" s="53"/>
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -5222,20 +5280,21 @@
       <c r="C12" t="s">
         <v>413</v>
       </c>
-      <c r="F12" t="s">
+      <c r="D12"/>
+      <c r="G12" t="s">
         <v>414</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>360</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="L12" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>139</v>
       </c>
@@ -5245,26 +5304,26 @@
       <c r="C13" s="10" t="s">
         <v>360</v>
       </c>
-      <c r="F13" t="s">
-        <v>360</v>
-      </c>
-      <c r="I13" s="11" t="s">
+      <c r="G13" t="s">
         <v>360</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="11" t="s">
         <v>360</v>
       </c>
-      <c r="N13" t="s">
+      <c r="L13" t="s">
+        <v>360</v>
+      </c>
+      <c r="O13" t="s">
         <v>423</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>33</v>
       </c>
@@ -5274,14 +5333,14 @@
       <c r="C14" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>375</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>394</v>
       </c>
@@ -5291,17 +5350,18 @@
       <c r="C15" t="s">
         <v>396</v>
       </c>
-      <c r="F15" t="s">
+      <c r="D15"/>
+      <c r="G15" t="s">
         <v>395</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>377</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -5311,20 +5371,21 @@
       <c r="C16" t="s">
         <v>360</v>
       </c>
-      <c r="F16" t="s">
+      <c r="D16"/>
+      <c r="G16" t="s">
         <v>360</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>360</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>420</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -5334,14 +5395,15 @@
       <c r="C17" t="s">
         <v>422</v>
       </c>
-      <c r="K17" t="s">
+      <c r="D17"/>
+      <c r="L17" t="s">
         <v>375</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>401</v>
       </c>
@@ -5351,20 +5413,23 @@
       <c r="C18" t="s">
         <v>402</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D18" t="s">
+        <v>437</v>
+      </c>
+      <c r="G18" t="s">
         <v>411</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="H18" s="68" t="s">
+      <c r="I18" s="57" t="s">
         <v>426</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>387</v>
       </c>
@@ -5374,31 +5439,34 @@
       <c r="C19" t="s">
         <v>405</v>
       </c>
-      <c r="F19" t="s">
+      <c r="D19" t="s">
+        <v>438</v>
+      </c>
+      <c r="G19" t="s">
         <v>378</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="J19" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>377</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>139</v>
       </c>
       <c r="B20" t="s">
         <v>407</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -5408,145 +5476,148 @@
       <c r="C21" t="s">
         <v>410</v>
       </c>
-      <c r="K21" t="s">
+      <c r="D21" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="L21" t="s">
         <v>375</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C1048576 I1:I1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="134" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 J1:J1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="135" priority="49" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 O1:O1048576 I1:I1048576">
-    <cfRule type="expression" dxfId="133" priority="46" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 P1:P1048576 J1:J1048576">
+    <cfRule type="expression" dxfId="134" priority="46" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="132" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="133" priority="43" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="131" priority="41" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
+    <cfRule type="expression" dxfId="132" priority="41" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:D1048576 G1:H1048576">
-    <cfRule type="expression" dxfId="130" priority="39" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E1048576 H1:I1048576">
+    <cfRule type="expression" dxfId="131" priority="39" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="129" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="130" priority="34" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="128" priority="24" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:G1048576 B1:B1048576">
+    <cfRule type="expression" dxfId="129" priority="24" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="127" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576">
+    <cfRule type="expression" dxfId="128" priority="18" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="20" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="22" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="124" priority="16" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:O1048576 B1:B1048576">
+    <cfRule type="expression" dxfId="125" priority="16" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="123" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="124" priority="14" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="122" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="123" priority="10" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="121" priority="8" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:D1048576">
+    <cfRule type="expression" dxfId="122" priority="8" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="120" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:X1048576">
+    <cfRule type="expression" dxfId="121" priority="2" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="5" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="9" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="11" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="15" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="17" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="19" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="21" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="23" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="25" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="28" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="35" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="40" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="42" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="44" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="45" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="47" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="48" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="50" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="101" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="3" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B1048576 G1:G1048576">
+    <cfRule type="expression" dxfId="101" priority="1" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5558,11 +5629,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5570,11 +5641,12 @@
     <col min="1" max="1" width="15.5" style="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="14.5" style="15" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="10.83203125" style="15" collapsed="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1" collapsed="1"/>
+    <col min="4" max="4" width="39.6640625" style="15" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="15" collapsed="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -5584,14 +5656,17 @@
       <c r="C1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>21</v>
       </c>
@@ -5601,8 +5676,11 @@
       <c r="C2" s="16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="16" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>21</v>
       </c>
@@ -5612,8 +5690,11 @@
       <c r="C3" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="16" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>379</v>
       </c>
@@ -5623,11 +5704,14 @@
       <c r="C4" t="s">
         <v>380</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>379</v>
       </c>
@@ -5637,11 +5721,14 @@
       <c r="C5" t="s">
         <v>382</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s">
+        <v>430</v>
+      </c>
+      <c r="F5" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>379</v>
       </c>
@@ -5651,11 +5738,14 @@
       <c r="C6" t="s">
         <v>384</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F6" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>379</v>
       </c>
@@ -5665,23 +5755,29 @@
       <c r="C7" t="s">
         <v>386</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
+        <v>432</v>
+      </c>
+      <c r="F7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="B8" s="67">
+      <c r="B8" s="56">
         <v>0</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="55" t="s">
         <v>424</v>
       </c>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" s="55" t="s">
+        <v>433</v>
+      </c>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>379</v>
       </c>
@@ -5691,11 +5787,14 @@
       <c r="C9" t="s">
         <v>389</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="55" t="s">
+        <v>434</v>
+      </c>
+      <c r="F9" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>390</v>
       </c>
@@ -5705,8 +5804,9 @@
       <c r="C10" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>390</v>
       </c>
@@ -5716,8 +5816,9 @@
       <c r="C11" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>390</v>
       </c>
@@ -5727,8 +5828,9 @@
       <c r="C12" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>390</v>
       </c>
@@ -5738,8 +5840,9 @@
       <c r="C13" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>390</v>
       </c>
@@ -5748,6 +5851,9 @@
       </c>
       <c r="C14" t="s">
         <v>389</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
@@ -5759,14 +5865,19 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:H8 A10:H2001">
-    <cfRule type="expression" dxfId="99" priority="1">
+  <conditionalFormatting sqref="A2:I3 A10:I2001 A8:I8 A4:C7 E4:I7">
+    <cfRule type="expression" dxfId="100" priority="2">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:H9">
-    <cfRule type="expression" dxfId="0" priority="100">
+  <conditionalFormatting sqref="A9:I9">
+    <cfRule type="expression" dxfId="99" priority="101">
       <formula>NOT($A9=$A7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>NOT($A4=$A3)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5823,7 +5934,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2005041825</v>
+        <v>2005121928</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>360</v>
@@ -5858,22 +5969,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -6067,10 +6178,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="64" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="61"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -8860,10 +8971,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="62" t="s">
+      <c r="A83" s="65" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="63"/>
+      <c r="B83" s="66"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -10023,20 +10134,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="56"/>
+      <c r="B1" s="59"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="63"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -10111,28 +10222,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="65"/>
+      <c r="B1" s="68"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="60"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>